<commit_message>
added max return portfolio calc
</commit_message>
<xml_diff>
--- a/youtube.xlsx
+++ b/youtube.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6113f60f932799a7/1Evan/.eff_fron_spyder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{E14160CD-FFF5-4370-B3E6-1B33596AC807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12624AD8-3B6C-4D21-AD8F-C73D4B336B2B}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{E14160CD-FFF5-4370-B3E6-1B33596AC807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3B6B4FB-33FF-468E-A633-F775D99C0EDD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0%"/>
+    <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -123,20 +123,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -163,10 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,7 +566,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -595,7 +591,7 @@
         <v>39231</v>
       </c>
       <c r="B2" s="9">
-        <v>45065</v>
+        <v>45066</v>
       </c>
       <c r="C2" s="10">
         <v>3.6999999999999998E-2</v>

</xml_diff>